<commit_message>
Updated clue layout xcel sheet, had wrong door directions compared to config file
</commit_message>
<xml_diff>
--- a/Clue Layout.xlsx
+++ b/Clue Layout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="524" uniqueCount="51">
   <si>
     <t>C</t>
   </si>
@@ -54,9 +54,6 @@
     <t>C = Conservatory</t>
   </si>
   <si>
-    <t>CD</t>
-  </si>
-  <si>
     <t>RD</t>
   </si>
   <si>
@@ -162,10 +159,16 @@
     <t>SL</t>
   </si>
   <si>
-    <t>OU</t>
-  </si>
-  <si>
     <t>Light Purple: adjacency list tests, only walkways as locations</t>
+  </si>
+  <si>
+    <t>HU</t>
+  </si>
+  <si>
+    <t>CR</t>
+  </si>
+  <si>
+    <t>OL</t>
   </si>
 </sst>
 </file>
@@ -181,7 +184,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,12 +241,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="-0.24994659260841701"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor rgb="FFCCCCFF"/>
       </patternFill>
@@ -256,8 +253,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59996337778862885"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor rgb="FFCCCCFF"/>
       </patternFill>
     </fill>
   </fills>
@@ -325,7 +322,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -365,9 +362,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -739,11 +733,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y75"/>
+  <dimension ref="A1:AA75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -752,7 +744,7 @@
     <col min="26" max="257" width="4.28515625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -771,7 +763,7 @@
       <c r="F1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="17" t="s">
+      <c r="G1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H1" s="1" t="s">
@@ -789,7 +781,7 @@
       <c r="L1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="17" t="s">
+      <c r="M1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -819,11 +811,14 @@
       <c r="V1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="W1" s="15" t="s">
+      <c r="W1" s="14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -893,16 +888,19 @@
       <c r="W2" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>0</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>0</v>
@@ -920,10 +918,10 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>2</v>
@@ -935,7 +933,7 @@
         <v>1</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="O3" s="1" t="s">
         <v>3</v>
@@ -959,16 +957,19 @@
         <v>4</v>
       </c>
       <c r="V3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="Y3" s="3" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>0</v>
       </c>
@@ -987,7 +988,7 @@
       <c r="F4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
@@ -1005,7 +1006,7 @@
       <c r="L4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="2" t="s">
         <v>1</v>
       </c>
       <c r="N4" s="1" t="s">
@@ -1041,8 +1042,11 @@
       <c r="Y4" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -1053,7 +1057,7 @@
         <v>0</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>1</v>
@@ -1068,7 +1072,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J5" s="1" t="s">
         <v>2</v>
@@ -1104,7 +1108,7 @@
         <v>1</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="V5" s="1" t="s">
         <v>4</v>
@@ -1113,10 +1117,13 @@
         <v>4</v>
       </c>
       <c r="Y5" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="AA5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>1</v>
       </c>
@@ -1126,7 +1133,7 @@
       <c r="C6" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
@@ -1162,7 +1169,7 @@
       <c r="O6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P6" s="16" t="s">
+      <c r="P6" s="15" t="s">
         <v>7</v>
       </c>
       <c r="Q6" s="1" t="s">
@@ -1187,971 +1194,1013 @@
         <v>4</v>
       </c>
       <c r="Y6" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="4" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AA7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="K8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="L8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="M8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="N8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="O8" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J8" s="5" t="s">
+      <c r="P8" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="S8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="T8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="5" t="s">
+      <c r="U8" s="16" t="s">
+        <v>48</v>
+      </c>
+      <c r="V8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N8" s="5" t="s">
+      <c r="W8" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O8" s="5" t="s">
+      <c r="Y8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="AA8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P8" s="5" t="s">
+      <c r="S9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y8" s="4" t="s">
+      <c r="T9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W9" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y9" s="4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
+      <c r="AA9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="K10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="L10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="M10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="N10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="O10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J9" s="5" t="s">
+      <c r="P10" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q10" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R10" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="S10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="T10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="L9" s="5" t="s">
+      <c r="U10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M9" s="5" t="s">
+      <c r="V10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="N9" s="5" t="s">
+      <c r="W10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="5" t="s">
+      <c r="Y10" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="AA10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P11" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q11" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="S11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="P9" s="5" t="s">
+      <c r="T11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q9" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y9" s="4" t="s">
+      <c r="U11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W11" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y11" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="M12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="P12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W12" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y12" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="W13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y13" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="AA13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
+      <c r="F14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="N14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="O14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="P14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W14" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="T15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="U15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="W15" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O16" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R16" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="T16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O17" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W17" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O18" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W18" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA18">
         <v>17</v>
       </c>
-      <c r="B10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J10" s="5" t="s">
+    </row>
+    <row r="19" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="P19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R19" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="T19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W19" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA19">
         <v>18</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q10" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R10" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="S10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y10" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q11" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R11" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="S11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="V11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W11" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y11" s="4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="12" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G12" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="L12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="N12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="O12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="P12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="Q12" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="13" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="T13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="W13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="Y13" s="6" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="14" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="M14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="N14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="O14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="P14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V14" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W14" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>1</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="M15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="U15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="V15" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="W15" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R16" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S16" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="T16" s="1" t="s">
+    </row>
+    <row r="20" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U16" s="1" t="s">
+      <c r="B20" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="V16" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W16" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="17" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="J17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O17" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V17" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W17" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="G18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R18" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W18" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="19" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="L19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O19" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="P19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R19" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U19" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W19" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="20" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>31</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>1</v>
@@ -2160,223 +2209,278 @@
         <v>1</v>
       </c>
       <c r="I20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O20" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R20" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="T20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="U20" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="V20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L20" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M20" s="1" t="s">
+      <c r="W20" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="AA20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="T21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="P20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R20" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S20" s="1" t="s">
+      <c r="U21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="W21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="B22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="C22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="D22" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="F22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="R22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="S22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="T22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="U22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="V22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="W22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O21" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R21" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W21" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="G22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="H22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="K22" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="S22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="T22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="V22" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="W22" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="8"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="8"/>
-      <c r="M23" s="8"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
+      <c r="AA22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>0</v>
+      </c>
+      <c r="B23" s="8">
+        <v>1</v>
+      </c>
+      <c r="C23" s="8">
+        <v>2</v>
+      </c>
+      <c r="D23" s="8">
+        <v>3</v>
+      </c>
+      <c r="E23" s="8">
+        <v>4</v>
+      </c>
+      <c r="F23" s="8">
+        <v>5</v>
+      </c>
+      <c r="G23" s="8">
+        <v>6</v>
+      </c>
+      <c r="H23" s="8">
+        <v>7</v>
+      </c>
+      <c r="I23" s="8">
+        <v>8</v>
+      </c>
+      <c r="J23" s="8">
+        <v>9</v>
+      </c>
+      <c r="K23" s="8">
+        <v>10</v>
+      </c>
+      <c r="L23" s="8">
+        <v>11</v>
+      </c>
+      <c r="M23" s="8">
+        <v>12</v>
+      </c>
+      <c r="N23" s="8">
+        <v>13</v>
+      </c>
+      <c r="O23" s="8">
+        <v>14</v>
+      </c>
+      <c r="P23" s="8">
+        <v>15</v>
+      </c>
+      <c r="Q23" s="8">
+        <v>16</v>
+      </c>
+      <c r="R23" s="8">
+        <v>17</v>
+      </c>
+      <c r="S23" s="8">
+        <v>18</v>
+      </c>
+      <c r="T23" s="8">
+        <v>19</v>
+      </c>
+      <c r="U23" s="8">
+        <v>20</v>
+      </c>
+      <c r="V23" s="8">
+        <v>21</v>
+      </c>
+      <c r="W23" s="8">
+        <v>22</v>
+      </c>
       <c r="X23" s="8"/>
       <c r="Y23" s="8"/>
     </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -2403,9 +2507,9 @@
       <c r="X24" s="8"/>
       <c r="Y24" s="8"/>
     </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -2432,9 +2536,9 @@
       <c r="X25" s="8"/>
       <c r="Y25" s="8"/>
     </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A26" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -2461,9 +2565,9 @@
       <c r="X26" s="8"/>
       <c r="Y26" s="8"/>
     </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A27" s="9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B27" s="8"/>
       <c r="C27" s="8"/>
@@ -2490,9 +2594,9 @@
       <c r="X27" s="8"/>
       <c r="Y27" s="8"/>
     </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A28" s="9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -2519,9 +2623,9 @@
       <c r="X28" s="8"/>
       <c r="Y28" s="8"/>
     </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A29" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
@@ -2548,9 +2652,9 @@
       <c r="X29" s="8"/>
       <c r="Y29" s="8"/>
     </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A30" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B30" s="8"/>
       <c r="C30" s="8"/>
@@ -2577,7 +2681,7 @@
       <c r="X30" s="8"/>
       <c r="Y30" s="8"/>
     </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A31" s="8"/>
       <c r="B31" s="8"/>
       <c r="C31" s="8"/>
@@ -2604,7 +2708,7 @@
       <c r="X31" s="8"/>
       <c r="Y31" s="8"/>
     </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A32" s="8"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>

</xml_diff>